<commit_message>
Pr quadratic parameters plotted
</commit_message>
<xml_diff>
--- a/src/prommis/solvent_extraction/feed_phi_parameters.xlsx
+++ b/src/prommis/solvent_extraction/feed_phi_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad00105\Desktop\Model_software\prommis\src\prommis\solvent_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9A40CF-0B96-4FF6-80BD-974155CB487F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871A7526-91F9-4411-9BEE-E2172B82B712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All HCl data" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,13 @@
     <sheet name="5 M HCl alpha values" sheetId="6" r:id="rId6"/>
     <sheet name="1 M HCl alpha values" sheetId="7" r:id="rId7"/>
     <sheet name="3 M HCl alpha values" sheetId="8" r:id="rId8"/>
+    <sheet name="1 M HCl alt" sheetId="9" r:id="rId9"/>
+    <sheet name="1 M HCl alpha values alt" sheetId="10" r:id="rId10"/>
+    <sheet name="3 M HCl alt" sheetId="11" r:id="rId11"/>
+    <sheet name="3 M HCl alpha values alt" sheetId="12" r:id="rId12"/>
+    <sheet name="5 M HCl alt" sheetId="13" r:id="rId13"/>
+    <sheet name="5 M HCl alpha values alt" sheetId="14" r:id="rId14"/>
+    <sheet name="All HCl data alt" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="41">
   <si>
     <t>1 M HCl</t>
   </si>
@@ -172,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +212,27 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -214,7 +242,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -282,11 +310,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -300,6 +373,18 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -584,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,12 +691,15 @@
         <v>3</v>
       </c>
       <c r="B2">
+        <f>'1 M HCl'!B2</f>
         <v>-1.4905586399201599E-3</v>
       </c>
       <c r="C2">
+        <f>'3 M HCl'!B2</f>
         <v>2.288195142548257E-2</v>
       </c>
       <c r="D2">
+        <f>'5 M HCl'!B2</f>
         <v>-1.171821233261041E-2</v>
       </c>
     </row>
@@ -620,12 +708,15 @@
         <v>4</v>
       </c>
       <c r="B3">
+        <f>'1 M HCl'!B3</f>
         <v>3.9326962088979964E-3</v>
       </c>
       <c r="C3">
+        <f>'3 M HCl'!B3</f>
         <v>-5.2621551354364608E-3</v>
       </c>
       <c r="D3">
+        <f>'5 M HCl'!B3</f>
         <v>4.0968003381782053E-2</v>
       </c>
     </row>
@@ -634,12 +725,15 @@
         <v>5</v>
       </c>
       <c r="B4">
+        <f>'1 M HCl'!B4</f>
         <v>4.3597279239085477E-5</v>
       </c>
       <c r="C4">
+        <f>'3 M HCl'!B4</f>
         <v>1.40168129186233E-3</v>
       </c>
       <c r="D4">
+        <f>'5 M HCl'!B4</f>
         <v>-1.1640607133710261E-3</v>
       </c>
     </row>
@@ -648,12 +742,15 @@
         <v>6</v>
       </c>
       <c r="B5">
+        <f>'1 M HCl'!B5</f>
         <v>5.1521921712242901E-4</v>
       </c>
       <c r="C5">
+        <f>'3 M HCl'!B5</f>
         <v>8.3900563271528394E-3</v>
       </c>
       <c r="D5">
+        <f>'5 M HCl'!B5</f>
         <v>-4.9187766197291687E-3</v>
       </c>
     </row>
@@ -662,12 +759,15 @@
         <v>7</v>
       </c>
       <c r="B6">
+        <f>'1 M HCl'!B6</f>
         <v>7.5287793978559699E-4</v>
       </c>
       <c r="C6">
+        <f>'3 M HCl'!B6</f>
         <v>-2.110618497222582E-3</v>
       </c>
       <c r="D6">
+        <f>'5 M HCl'!B6</f>
         <v>1.6984243787947089E-2</v>
       </c>
     </row>
@@ -676,12 +776,15 @@
         <v>8</v>
       </c>
       <c r="B7">
+        <f>'1 M HCl'!B7</f>
         <v>1.154292868742197E-4</v>
       </c>
       <c r="C7">
+        <f>'3 M HCl'!B7</f>
         <v>8.0990711650242013E-4</v>
       </c>
       <c r="D7">
+        <f>'5 M HCl'!B7</f>
         <v>-1.330390472114545E-4</v>
       </c>
     </row>
@@ -690,12 +793,15 @@
         <v>9</v>
       </c>
       <c r="B8">
+        <f>'1 M HCl'!B8</f>
         <v>-3.0767595720595699E-6</v>
       </c>
       <c r="C8">
+        <f>'3 M HCl'!B8</f>
         <v>1.582894215397936E-5</v>
       </c>
       <c r="D8">
+        <f>'5 M HCl'!B8</f>
         <v>-5.4793789548301881E-6</v>
       </c>
     </row>
@@ -704,12 +810,15 @@
         <v>10</v>
       </c>
       <c r="B9">
+        <f>'1 M HCl'!B9</f>
         <v>5.3553703317697434E-6</v>
       </c>
       <c r="C9">
+        <f>'3 M HCl'!B9</f>
         <v>-8.4306054549185673E-6</v>
       </c>
       <c r="D9">
+        <f>'5 M HCl'!B9</f>
         <v>2.3955526283429288E-5</v>
       </c>
     </row>
@@ -718,12 +827,15 @@
         <v>11</v>
       </c>
       <c r="B10">
+        <f>'1 M HCl'!B10</f>
         <v>-3.4607454270235722E-7</v>
       </c>
       <c r="C10">
+        <f>'3 M HCl'!B10</f>
         <v>1.9496068041048691E-6</v>
       </c>
       <c r="D10">
+        <f>'5 M HCl'!B10</f>
         <v>-4.6392668057313481E-7</v>
       </c>
     </row>
@@ -732,12 +844,15 @@
         <v>12</v>
       </c>
       <c r="B11">
+        <f>'1 M HCl'!B11</f>
         <v>-4.2969730262548678E-4</v>
       </c>
       <c r="C11">
+        <f>'3 M HCl'!B11</f>
         <v>2.9615323580125509E-2</v>
       </c>
       <c r="D11">
+        <f>'5 M HCl'!B11</f>
         <v>-3.1421505929986819E-2</v>
       </c>
     </row>
@@ -746,12 +861,15 @@
         <v>13</v>
       </c>
       <c r="B12">
+        <f>'1 M HCl'!B12</f>
         <v>2.884373546767586E-3</v>
       </c>
       <c r="C12">
+        <f>'3 M HCl'!B12</f>
         <v>-9.6935535027941697E-3</v>
       </c>
       <c r="D12">
+        <f>'5 M HCl'!B12</f>
         <v>5.9197709052540133E-2</v>
       </c>
     </row>
@@ -760,12 +878,15 @@
         <v>14</v>
       </c>
       <c r="B13">
+        <f>'1 M HCl'!B13</f>
         <v>1.7785206879235109E-4</v>
       </c>
       <c r="C13">
+        <f>'3 M HCl'!B13</f>
         <v>2.1935632069776259E-3</v>
       </c>
       <c r="D13">
+        <f>'5 M HCl'!B13</f>
         <v>-1.118983944786452E-3</v>
       </c>
     </row>
@@ -774,12 +895,15 @@
         <v>15</v>
       </c>
       <c r="B14">
+        <f>'1 M HCl'!B14</f>
         <v>-5.4686500622420217E-3</v>
       </c>
       <c r="C14">
+        <f>'3 M HCl'!B14</f>
         <v>2.093956992689348E-2</v>
       </c>
       <c r="D14">
+        <f>'5 M HCl'!B14</f>
         <v>-8.8850982471848361E-3</v>
       </c>
     </row>
@@ -788,12 +912,15 @@
         <v>16</v>
       </c>
       <c r="B15">
+        <f>'1 M HCl'!B15</f>
         <v>9.824655350660726E-3</v>
       </c>
       <c r="C15">
+        <f>'3 M HCl'!B15</f>
         <v>-5.9727117249168031E-3</v>
       </c>
       <c r="D15">
+        <f>'5 M HCl'!B15</f>
         <v>3.2541123392962133E-2</v>
       </c>
     </row>
@@ -802,12 +929,15 @@
         <v>17</v>
       </c>
       <c r="B16">
+        <f>'1 M HCl'!B16</f>
         <v>-6.3461878216389646E-4</v>
       </c>
       <c r="C16">
+        <f>'3 M HCl'!B16</f>
         <v>1.27818470749062E-3</v>
       </c>
       <c r="D16">
+        <f>'5 M HCl'!B16</f>
         <v>-9.4988623471918576E-4</v>
       </c>
     </row>
@@ -816,12 +946,15 @@
         <v>18</v>
       </c>
       <c r="B17">
+        <f>'1 M HCl'!B17</f>
         <v>-2.750422316040336E-3</v>
       </c>
       <c r="C17">
+        <f>'3 M HCl'!B17</f>
         <v>1.016738956888703E-2</v>
       </c>
       <c r="D17">
+        <f>'5 M HCl'!B17</f>
         <v>-4.7679024066807326E-3</v>
       </c>
     </row>
@@ -830,12 +963,15 @@
         <v>19</v>
       </c>
       <c r="B18">
+        <f>'1 M HCl'!B18</f>
         <v>5.0783910935285814E-3</v>
       </c>
       <c r="C18">
+        <f>'3 M HCl'!B18</f>
         <v>-3.417155883653046E-3</v>
       </c>
       <c r="D18">
+        <f>'5 M HCl'!B18</f>
         <v>1.6155366435682491E-2</v>
       </c>
     </row>
@@ -844,12 +980,15 @@
         <v>20</v>
       </c>
       <c r="B19">
+        <f>'1 M HCl'!B19</f>
         <v>-3.7269420017426049E-4</v>
       </c>
       <c r="C19">
+        <f>'3 M HCl'!B19</f>
         <v>7.0384820140937234E-4</v>
       </c>
       <c r="D19">
+        <f>'5 M HCl'!B19</f>
         <v>-4.3377288836695158E-4</v>
       </c>
     </row>
@@ -858,12 +997,15 @@
         <v>21</v>
       </c>
       <c r="B20">
+        <f>'1 M HCl'!B20</f>
         <v>-6.4495274833007016E-3</v>
       </c>
       <c r="C20">
+        <f>'3 M HCl'!B20</f>
         <v>0.12982034907180079</v>
       </c>
       <c r="D20">
+        <f>'5 M HCl'!B20</f>
         <v>-0.19275700643109039</v>
       </c>
     </row>
@@ -872,12 +1014,15 @@
         <v>22</v>
       </c>
       <c r="B21">
+        <f>'1 M HCl'!B21</f>
         <v>1.9482783915760801E-2</v>
       </c>
       <c r="C21">
+        <f>'3 M HCl'!B21</f>
         <v>-4.0828033403723499E-2</v>
       </c>
       <c r="D21">
+        <f>'5 M HCl'!B21</f>
         <v>0.39694493563632072</v>
       </c>
     </row>
@@ -886,12 +1031,15 @@
         <v>23</v>
       </c>
       <c r="B22">
+        <f>'1 M HCl'!B22</f>
         <v>3.0187497310265861E-4</v>
       </c>
       <c r="C22">
+        <f>'3 M HCl'!B22</f>
         <v>8.9878701541057267E-3</v>
       </c>
       <c r="D22">
+        <f>'5 M HCl'!B22</f>
         <v>-2.940745455829458E-2</v>
       </c>
     </row>
@@ -900,12 +1048,15 @@
         <v>24</v>
       </c>
       <c r="B23">
+        <f>'1 M HCl'!B23</f>
         <v>-3.1088032144060679E-5</v>
       </c>
       <c r="C23">
+        <f>'3 M HCl'!B23</f>
         <v>8.6896732300363052E-5</v>
       </c>
       <c r="D23">
+        <f>'5 M HCl'!B23</f>
         <v>-3.8372115959739842E-5</v>
       </c>
     </row>
@@ -914,12 +1065,15 @@
         <v>25</v>
       </c>
       <c r="B24">
+        <f>'1 M HCl'!B24</f>
         <v>5.530378004203219E-5</v>
       </c>
       <c r="C24">
+        <f>'3 M HCl'!B24</f>
         <v>-3.049641118800322E-5</v>
       </c>
       <c r="D24">
+        <f>'5 M HCl'!B24</f>
         <v>1.266534148975326E-4</v>
       </c>
     </row>
@@ -928,16 +1082,2669 @@
         <v>26</v>
       </c>
       <c r="B25">
+        <f>'1 M HCl'!B25</f>
         <v>-4.0995377727066988E-6</v>
       </c>
       <c r="C25">
+        <f>'3 M HCl'!B25</f>
         <v>7.1708081920925164E-6</v>
       </c>
       <c r="D25">
+        <f>'5 M HCl'!B25</f>
         <v>-3.387408066091318E-6</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:C65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.9</v>
+      </c>
+      <c r="C2">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.9</v>
+      </c>
+      <c r="C4">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.9</v>
+      </c>
+      <c r="C5">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.9</v>
+      </c>
+      <c r="C6">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.9</v>
+      </c>
+      <c r="C7">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>0.9</v>
+      </c>
+      <c r="C8">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.9</v>
+      </c>
+      <c r="C9">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0.9</v>
+      </c>
+      <c r="C11">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.9</v>
+      </c>
+      <c r="C12">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>0.9</v>
+      </c>
+      <c r="C13">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>0.9</v>
+      </c>
+      <c r="C14">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>0.9</v>
+      </c>
+      <c r="C15">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>0.9</v>
+      </c>
+      <c r="C16">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>0.9</v>
+      </c>
+      <c r="C17">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>0.9</v>
+      </c>
+      <c r="C18">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>0.9</v>
+      </c>
+      <c r="C19">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>0.9</v>
+      </c>
+      <c r="C20">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>0.9</v>
+      </c>
+      <c r="C21">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <v>0.9</v>
+      </c>
+      <c r="C22">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>42</v>
+      </c>
+      <c r="B23">
+        <v>0.9</v>
+      </c>
+      <c r="C23">
+        <v>2.551366584794807E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <v>1.8</v>
+      </c>
+      <c r="C24">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>1.8</v>
+      </c>
+      <c r="C25">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>1.8</v>
+      </c>
+      <c r="C26">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>1.8</v>
+      </c>
+      <c r="C27">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>1.8</v>
+      </c>
+      <c r="C28">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>1.8</v>
+      </c>
+      <c r="C29">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>56</v>
+      </c>
+      <c r="B30">
+        <v>1.8</v>
+      </c>
+      <c r="C30">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>58</v>
+      </c>
+      <c r="B31">
+        <v>1.8</v>
+      </c>
+      <c r="C31">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>1.8</v>
+      </c>
+      <c r="C32">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>62</v>
+      </c>
+      <c r="B33">
+        <v>1.8</v>
+      </c>
+      <c r="C33">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>63</v>
+      </c>
+      <c r="B34">
+        <v>1.8</v>
+      </c>
+      <c r="C34">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>65</v>
+      </c>
+      <c r="B35">
+        <v>1.8</v>
+      </c>
+      <c r="C35">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>67</v>
+      </c>
+      <c r="B36">
+        <v>1.8</v>
+      </c>
+      <c r="C36">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>69</v>
+      </c>
+      <c r="B37">
+        <v>1.8</v>
+      </c>
+      <c r="C37">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>71</v>
+      </c>
+      <c r="B38">
+        <v>1.8</v>
+      </c>
+      <c r="C38">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>72</v>
+      </c>
+      <c r="B39">
+        <v>1.8</v>
+      </c>
+      <c r="C39">
+        <v>5.4401769767733286E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>74</v>
+      </c>
+      <c r="B40">
+        <v>2.7</v>
+      </c>
+      <c r="C40">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>76</v>
+      </c>
+      <c r="B41">
+        <v>2.7</v>
+      </c>
+      <c r="C41">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>78</v>
+      </c>
+      <c r="B42">
+        <v>2.7</v>
+      </c>
+      <c r="C42">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>80</v>
+      </c>
+      <c r="B43">
+        <v>2.7</v>
+      </c>
+      <c r="C43">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>82</v>
+      </c>
+      <c r="B44">
+        <v>2.7</v>
+      </c>
+      <c r="C44">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>84</v>
+      </c>
+      <c r="B45">
+        <v>2.7</v>
+      </c>
+      <c r="C45">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>86</v>
+      </c>
+      <c r="B46">
+        <v>2.7</v>
+      </c>
+      <c r="C46">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>88</v>
+      </c>
+      <c r="B47">
+        <v>2.7</v>
+      </c>
+      <c r="C47">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>90</v>
+      </c>
+      <c r="B48">
+        <v>2.7</v>
+      </c>
+      <c r="C48">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>92</v>
+      </c>
+      <c r="B49">
+        <v>2.7</v>
+      </c>
+      <c r="C49">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>94</v>
+      </c>
+      <c r="B50">
+        <v>2.7</v>
+      </c>
+      <c r="C50">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>96</v>
+      </c>
+      <c r="B51">
+        <v>2.7</v>
+      </c>
+      <c r="C51">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>98</v>
+      </c>
+      <c r="B52">
+        <v>2.7</v>
+      </c>
+      <c r="C52">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>100</v>
+      </c>
+      <c r="B53">
+        <v>2.7</v>
+      </c>
+      <c r="C53">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>102</v>
+      </c>
+      <c r="B54">
+        <v>2.7</v>
+      </c>
+      <c r="C54">
+        <v>8.671589037918077E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>104</v>
+      </c>
+      <c r="B55">
+        <v>4.5</v>
+      </c>
+      <c r="C55">
+        <v>1.6162218167706251E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>106</v>
+      </c>
+      <c r="B56">
+        <v>4.5</v>
+      </c>
+      <c r="C56">
+        <v>1.6162218167706251E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>108</v>
+      </c>
+      <c r="B57">
+        <v>4.5</v>
+      </c>
+      <c r="C57">
+        <v>1.6162218167706251E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>110</v>
+      </c>
+      <c r="B58">
+        <v>4.5</v>
+      </c>
+      <c r="C58">
+        <v>1.6162218167706251E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>112</v>
+      </c>
+      <c r="B59">
+        <v>4.5</v>
+      </c>
+      <c r="C59">
+        <v>1.6162218167706251E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>114</v>
+      </c>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>4.0884320202585651E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>116</v>
+      </c>
+      <c r="B61">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>4.0884320202585651E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>117</v>
+      </c>
+      <c r="B62">
+        <v>9</v>
+      </c>
+      <c r="C62">
+        <v>4.0884320202585651E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>119</v>
+      </c>
+      <c r="B63">
+        <v>9</v>
+      </c>
+      <c r="C63">
+        <v>4.0884320202585651E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>121</v>
+      </c>
+      <c r="B64">
+        <v>9</v>
+      </c>
+      <c r="C64">
+        <v>4.0884320202585651E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>122</v>
+      </c>
+      <c r="B65">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>4.0884320202585651E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1.5991219281900719E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1.220271587799641E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>6.3626344660642174E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>5.9218046864101858E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>2.5506950329193949E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>4.848064317978129E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>5.2188955127484069E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>5.732796095388899E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1.730635345247275E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>3.09733527395539E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>7.8628528506205682E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1.266812756636288E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>9.1324337772476677E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>4.5029622360397468E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>5.5923757900509857E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>3.4012382976617791E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>2.1951216205647541E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>7.6010193297241901E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>3.3975311662409062E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>3.186440637807876E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>4.7148213816750597E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>4.2752898438335413E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>2.626269985095406E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:C58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.9</v>
+      </c>
+      <c r="C2">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.9</v>
+      </c>
+      <c r="C4">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.9</v>
+      </c>
+      <c r="C5">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.9</v>
+      </c>
+      <c r="C6">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.9</v>
+      </c>
+      <c r="C7">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>0.9</v>
+      </c>
+      <c r="C8">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.9</v>
+      </c>
+      <c r="C9">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0.9</v>
+      </c>
+      <c r="C11">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>0.9</v>
+      </c>
+      <c r="C12">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0.9</v>
+      </c>
+      <c r="C13">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>0.9</v>
+      </c>
+      <c r="C14">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>0.9</v>
+      </c>
+      <c r="C15">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>0.9</v>
+      </c>
+      <c r="C16">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>0.9</v>
+      </c>
+      <c r="C17">
+        <v>1.6616417116553889E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>1.8</v>
+      </c>
+      <c r="C18">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>1.8</v>
+      </c>
+      <c r="C19">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>1.8</v>
+      </c>
+      <c r="C20">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>1.8</v>
+      </c>
+      <c r="C21">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>1.8</v>
+      </c>
+      <c r="C22">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>1.8</v>
+      </c>
+      <c r="C23">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>1.8</v>
+      </c>
+      <c r="C24">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>1.8</v>
+      </c>
+      <c r="C25">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>45</v>
+      </c>
+      <c r="B26">
+        <v>1.8</v>
+      </c>
+      <c r="C26">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>1.8</v>
+      </c>
+      <c r="C27">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>1.8</v>
+      </c>
+      <c r="C28">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>51</v>
+      </c>
+      <c r="B29">
+        <v>1.8</v>
+      </c>
+      <c r="C29">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>53</v>
+      </c>
+      <c r="B30">
+        <v>1.8</v>
+      </c>
+      <c r="C30">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>55</v>
+      </c>
+      <c r="B31">
+        <v>1.8</v>
+      </c>
+      <c r="C31">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>57</v>
+      </c>
+      <c r="B32">
+        <v>1.8</v>
+      </c>
+      <c r="C32">
+        <v>1.8272361734709461E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>59</v>
+      </c>
+      <c r="B33">
+        <v>2.7</v>
+      </c>
+      <c r="C33">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>61</v>
+      </c>
+      <c r="B34">
+        <v>2.7</v>
+      </c>
+      <c r="C34">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>63</v>
+      </c>
+      <c r="B35">
+        <v>2.7</v>
+      </c>
+      <c r="C35">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>65</v>
+      </c>
+      <c r="B36">
+        <v>2.7</v>
+      </c>
+      <c r="C36">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>66</v>
+      </c>
+      <c r="B37">
+        <v>2.7</v>
+      </c>
+      <c r="C37">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>68</v>
+      </c>
+      <c r="B38">
+        <v>2.7</v>
+      </c>
+      <c r="C38">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>70</v>
+      </c>
+      <c r="B39">
+        <v>2.7</v>
+      </c>
+      <c r="C39">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>72</v>
+      </c>
+      <c r="B40">
+        <v>2.7</v>
+      </c>
+      <c r="C40">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>74</v>
+      </c>
+      <c r="B41">
+        <v>2.7</v>
+      </c>
+      <c r="C41">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>76</v>
+      </c>
+      <c r="B42">
+        <v>2.7</v>
+      </c>
+      <c r="C42">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>78</v>
+      </c>
+      <c r="B43">
+        <v>2.7</v>
+      </c>
+      <c r="C43">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>80</v>
+      </c>
+      <c r="B44">
+        <v>2.7</v>
+      </c>
+      <c r="C44">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>81</v>
+      </c>
+      <c r="B45">
+        <v>2.7</v>
+      </c>
+      <c r="C45">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>83</v>
+      </c>
+      <c r="B46">
+        <v>2.7</v>
+      </c>
+      <c r="C46">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>85</v>
+      </c>
+      <c r="B47">
+        <v>2.7</v>
+      </c>
+      <c r="C47">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>87</v>
+      </c>
+      <c r="B48">
+        <v>2.7</v>
+      </c>
+      <c r="C48">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>89</v>
+      </c>
+      <c r="B49">
+        <v>2.7</v>
+      </c>
+      <c r="C49">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>90</v>
+      </c>
+      <c r="B50">
+        <v>2.7</v>
+      </c>
+      <c r="C50">
+        <v>2.095905313636744E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>92</v>
+      </c>
+      <c r="B51">
+        <v>4.5</v>
+      </c>
+      <c r="C51">
+        <v>2.9424676290190601E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>94</v>
+      </c>
+      <c r="B52">
+        <v>4.5</v>
+      </c>
+      <c r="C52">
+        <v>2.9424676290190601E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>96</v>
+      </c>
+      <c r="B53">
+        <v>4.5</v>
+      </c>
+      <c r="C53">
+        <v>2.9424676290190601E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
+        <v>98</v>
+      </c>
+      <c r="B54">
+        <v>4.5</v>
+      </c>
+      <c r="C54">
+        <v>2.9424676290190601E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
+        <v>100</v>
+      </c>
+      <c r="B55">
+        <v>4.5</v>
+      </c>
+      <c r="C55">
+        <v>2.9424676290190601E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>102</v>
+      </c>
+      <c r="B56">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>6.8626802886040561E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
+        <v>104</v>
+      </c>
+      <c r="B57">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>6.8626802886040561E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>105</v>
+      </c>
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>6.8626802886040561E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8.5000525823965875E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2.9979648216683339E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4.9323484169988942E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2.1343870827034671E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1.276397855174677E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>4.7755638940740131E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1.146045327086256E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1.8989173694339169E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>2.214369113165429E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>9.4530026226597043E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2.6656702132464419E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>5.1178348783042886E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>4.8393554583343738E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>2.407490130647896E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>2.8640656934426852E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>2.30969728800637E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>1.1728950131281359E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>2.0379996577103051E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>0.33724502838904841</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>7.3325816349995604E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>2.3417686804827409E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>1.878268363137152E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>9.0979419837597709E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>1.745512472654276E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.7</v>
+      </c>
+      <c r="C2">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2.7</v>
+      </c>
+      <c r="C3">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2.7</v>
+      </c>
+      <c r="C4">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2.7</v>
+      </c>
+      <c r="C5">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2.7</v>
+      </c>
+      <c r="C6">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0.9</v>
+      </c>
+      <c r="C7">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0.9</v>
+      </c>
+      <c r="C8">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>0.9</v>
+      </c>
+      <c r="C9">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>0.9</v>
+      </c>
+      <c r="C11">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>0.9</v>
+      </c>
+      <c r="C12">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>0.9</v>
+      </c>
+      <c r="C13">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>0.9</v>
+      </c>
+      <c r="C14">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>0.9</v>
+      </c>
+      <c r="C15">
+        <v>2.8231208875031569E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>1.8</v>
+      </c>
+      <c r="C16">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>1.8</v>
+      </c>
+      <c r="C17">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>1.8</v>
+      </c>
+      <c r="C18">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>1.8</v>
+      </c>
+      <c r="C19">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>1.8</v>
+      </c>
+      <c r="C20">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>1.8</v>
+      </c>
+      <c r="C21">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>1.8</v>
+      </c>
+      <c r="C22">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>61</v>
+      </c>
+      <c r="B23">
+        <v>1.8</v>
+      </c>
+      <c r="C23">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>1.8</v>
+      </c>
+      <c r="C24">
+        <v>5.6411452935377297E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>67</v>
+      </c>
+      <c r="B25">
+        <v>2.7</v>
+      </c>
+      <c r="C25">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>70</v>
+      </c>
+      <c r="B26">
+        <v>2.7</v>
+      </c>
+      <c r="C26">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>73</v>
+      </c>
+      <c r="B27">
+        <v>2.7</v>
+      </c>
+      <c r="C27">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>76</v>
+      </c>
+      <c r="B28">
+        <v>2.7</v>
+      </c>
+      <c r="C28">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>79</v>
+      </c>
+      <c r="B29">
+        <v>2.7</v>
+      </c>
+      <c r="C29">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>82</v>
+      </c>
+      <c r="B30">
+        <v>2.7</v>
+      </c>
+      <c r="C30">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>85</v>
+      </c>
+      <c r="B31">
+        <v>2.7</v>
+      </c>
+      <c r="C31">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>88</v>
+      </c>
+      <c r="B32">
+        <v>2.7</v>
+      </c>
+      <c r="C32">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>91</v>
+      </c>
+      <c r="B33">
+        <v>2.7</v>
+      </c>
+      <c r="C33">
+        <v>8.5390737439276845E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>94</v>
+      </c>
+      <c r="B34">
+        <v>4.5</v>
+      </c>
+      <c r="C34">
+        <v>0.14574642777773739</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>97</v>
+      </c>
+      <c r="B35">
+        <v>4.5</v>
+      </c>
+      <c r="C35">
+        <v>0.14574642777773739</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>100</v>
+      </c>
+      <c r="B36">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>0.31061886138608069</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>101</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>0.31061886138608069</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2845A9-ED3B-45C6-BD16-F9799F59C8BC}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>'1 M HCl alt'!B2</f>
+        <v>5.1578619825110884E-6</v>
+      </c>
+      <c r="C2">
+        <f>'3 M HCl alt'!B2</f>
+        <v>1.5991219281900719E-2</v>
+      </c>
+      <c r="D2">
+        <f>'5 M HCl alt'!B2</f>
+        <v>8.5000525823965875E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>'1 M HCl alt'!B3</f>
+        <v>2.63878654247687E-3</v>
+      </c>
+      <c r="C3">
+        <f>'3 M HCl alt'!B3</f>
+        <v>1.220271587799641E-4</v>
+      </c>
+      <c r="D3">
+        <f>'5 M HCl alt'!B3</f>
+        <v>2.9979648216683339E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>'1 M HCl alt'!B4</f>
+        <v>2.1148251183100391E-4</v>
+      </c>
+      <c r="C4">
+        <f>'3 M HCl alt'!B4</f>
+        <v>6.3626344660642174E-4</v>
+      </c>
+      <c r="D4">
+        <f>'5 M HCl alt'!B4</f>
+        <v>4.9323484169988942E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f>'1 M HCl alt'!B5</f>
+        <v>5.2335662677863853E-4</v>
+      </c>
+      <c r="C5">
+        <f>'3 M HCl alt'!B5</f>
+        <v>5.9218046864101858E-3</v>
+      </c>
+      <c r="D5">
+        <f>'5 M HCl alt'!B5</f>
+        <v>2.1343870827034671E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f>'1 M HCl alt'!B6</f>
+        <v>7.4668008171754603E-4</v>
+      </c>
+      <c r="C6">
+        <f>'3 M HCl alt'!B6</f>
+        <v>2.5506950329193949E-5</v>
+      </c>
+      <c r="D6">
+        <f>'5 M HCl alt'!B6</f>
+        <v>1.276397855174677E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>'1 M HCl alt'!B7</f>
+        <v>1.161771101842082E-4</v>
+      </c>
+      <c r="C7">
+        <f>'3 M HCl alt'!B7</f>
+        <v>4.848064317978129E-4</v>
+      </c>
+      <c r="D7">
+        <f>'5 M HCl alt'!B7</f>
+        <v>4.7755638940740131E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f>'1 M HCl alt'!B8</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>'3 M HCl alt'!B8</f>
+        <v>5.2188955127484069E-6</v>
+      </c>
+      <c r="D8">
+        <f>'5 M HCl alt'!B8</f>
+        <v>1.146045327086256E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f>'1 M HCl alt'!B9</f>
+        <v>2.5019407715950622E-6</v>
+      </c>
+      <c r="C9">
+        <f>'3 M HCl alt'!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>'5 M HCl alt'!B9</f>
+        <v>1.8989173694339169E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <f>'1 M HCl alt'!B10</f>
+        <v>2.644565999336859E-8</v>
+      </c>
+      <c r="C10">
+        <f>'3 M HCl alt'!B10</f>
+        <v>5.732796095388899E-7</v>
+      </c>
+      <c r="D10">
+        <f>'5 M HCl alt'!B10</f>
+        <v>2.214369113165429E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f>'1 M HCl alt'!B11</f>
+        <v>6.2380944902054969E-7</v>
+      </c>
+      <c r="C11">
+        <f>'3 M HCl alt'!B11</f>
+        <v>1.730635345247275E-2</v>
+      </c>
+      <c r="D11">
+        <f>'5 M HCl alt'!B11</f>
+        <v>9.4530026226597043E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>'1 M HCl alt'!B12</f>
+        <v>2.4974233093713648E-3</v>
+      </c>
+      <c r="C12">
+        <f>'3 M HCl alt'!B12</f>
+        <v>3.09733527395539E-6</v>
+      </c>
+      <c r="D12">
+        <f>'5 M HCl alt'!B12</f>
+        <v>2.6656702132464419E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <f>'1 M HCl alt'!B13</f>
+        <v>2.292482371398744E-4</v>
+      </c>
+      <c r="C13">
+        <f>'3 M HCl alt'!B13</f>
+        <v>7.8628528506205682E-4</v>
+      </c>
+      <c r="D13">
+        <f>'5 M HCl alt'!B13</f>
+        <v>5.1178348783042886E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <f>'1 M HCl alt'!B14</f>
+        <v>1.377003217218972E-6</v>
+      </c>
+      <c r="C14">
+        <f>'3 M HCl alt'!B14</f>
+        <v>1.266812756636288E-2</v>
+      </c>
+      <c r="D14">
+        <f>'5 M HCl alt'!B14</f>
+        <v>4.8393554583343738E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <f>'1 M HCl alt'!B15</f>
+        <v>4.8761674856694238E-3</v>
+      </c>
+      <c r="C15">
+        <f>'3 M HCl alt'!B15</f>
+        <v>9.1324337772476677E-5</v>
+      </c>
+      <c r="D15">
+        <f>'5 M HCl alt'!B15</f>
+        <v>2.407490130647896E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <f>'1 M HCl alt'!B16</f>
+        <v>4.9939458882913702E-6</v>
+      </c>
+      <c r="C16">
+        <f>'3 M HCl alt'!B16</f>
+        <v>4.5029622360397468E-4</v>
+      </c>
+      <c r="D16">
+        <f>'5 M HCl alt'!B16</f>
+        <v>2.8640656934426852E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <f>'1 M HCl alt'!B17</f>
+        <v>1.765553348798137E-5</v>
+      </c>
+      <c r="C17">
+        <f>'3 M HCl alt'!B17</f>
+        <v>5.5923757900509857E-3</v>
+      </c>
+      <c r="D17">
+        <f>'5 M HCl alt'!B17</f>
+        <v>2.30969728800637E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <f>'1 M HCl alt'!B18</f>
+        <v>2.3916496029275582E-3</v>
+      </c>
+      <c r="C18">
+        <f>'3 M HCl alt'!B18</f>
+        <v>3.4012382976617791E-5</v>
+      </c>
+      <c r="D18">
+        <f>'5 M HCl alt'!B18</f>
+        <v>1.1728950131281359E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <f>'1 M HCl alt'!B19</f>
+        <v>6.899764397639642E-8</v>
+      </c>
+      <c r="C19">
+        <f>'3 M HCl alt'!B19</f>
+        <v>2.1951216205647541E-4</v>
+      </c>
+      <c r="D19">
+        <f>'5 M HCl alt'!B19</f>
+        <v>2.0379996577103051E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <f>'1 M HCl alt'!B20</f>
+        <v>1.8924511125910651E-6</v>
+      </c>
+      <c r="C20">
+        <f>'3 M HCl alt'!B20</f>
+        <v>7.6010193297241901E-2</v>
+      </c>
+      <c r="D20">
+        <f>'5 M HCl alt'!B20</f>
+        <v>0.33724502838904841</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <f>'1 M HCl alt'!B21</f>
+        <v>1.3691909307052859E-2</v>
+      </c>
+      <c r="C21">
+        <f>'3 M HCl alt'!B21</f>
+        <v>3.3975311662409062E-5</v>
+      </c>
+      <c r="D21">
+        <f>'5 M HCl alt'!B21</f>
+        <v>7.3325816349995604E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <f>'1 M HCl alt'!B22</f>
+        <v>1.072528274281055E-3</v>
+      </c>
+      <c r="C22">
+        <f>'3 M HCl alt'!B22</f>
+        <v>3.186440637807876E-3</v>
+      </c>
+      <c r="D22">
+        <f>'5 M HCl alt'!B22</f>
+        <v>2.3417686804827409E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <f>'1 M HCl alt'!B23</f>
+        <v>1.6835367235917532E-8</v>
+      </c>
+      <c r="C23">
+        <f>'3 M HCl alt'!B23</f>
+        <v>4.7148213816750597E-5</v>
+      </c>
+      <c r="D23">
+        <f>'5 M HCl alt'!B23</f>
+        <v>1.878268363137152E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <f>'1 M HCl alt'!B24</f>
+        <v>2.5236763457843789E-5</v>
+      </c>
+      <c r="C24">
+        <f>'3 M HCl alt'!B24</f>
+        <v>4.2752898438335413E-7</v>
+      </c>
+      <c r="D24">
+        <f>'5 M HCl alt'!B24</f>
+        <v>9.0979419837597709E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <f>'1 M HCl alt'!B25</f>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>'3 M HCl alt'!B25</f>
+        <v>2.626269985095406E-6</v>
+      </c>
+      <c r="D25">
+        <f>'5 M HCl alt'!B25</f>
+        <v>1.745512472654276E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1094,7 +3901,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3513,4 +6320,216 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>5.1578619825110884E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2.63878654247687E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2.1148251183100391E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>5.2335662677863853E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>7.4668008171754603E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1.161771101842082E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2.5019407715950622E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>2.644565999336859E-8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>6.2380944902054969E-7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2.4974233093713648E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>2.292482371398744E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1.377003217218972E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>4.8761674856694238E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>4.9939458882913702E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1.765553348798137E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>2.3916496029275582E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>6.899764397639642E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>1.8924511125910651E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>1.3691909307052859E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>1.072528274281055E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>1.6835367235917532E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>2.5236763457843789E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>